<commit_message>
Ajustando formato da Box - varias linhas no mesmo arqquivo
</commit_message>
<xml_diff>
--- a/xls2xml/sample/input_box_new.xlsx
+++ b/xls2xml/sample/input_box_new.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="474">
   <si>
     <t xml:space="preserve">Título Original</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t xml:space="preserve">E0BD54C5614CDAA111855B563DAB7A9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godzilla: King Of The Monsters 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">godzilla_king_otm_hd_net_evod_sub_ptbr2.ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godzilla: King Of The Monsters 3</t>
   </si>
   <si>
     <t xml:space="preserve">Billing Id</t>
@@ -1837,10 +1846,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IP2"/>
+  <dimension ref="A1:IP4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2346,17 +2355,269 @@
       </c>
       <c r="IO2" s="1"/>
     </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="P3" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="Q3" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AB3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AC3" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ3" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL3" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AO3" s="17" t="n">
+        <v>43726</v>
+      </c>
+      <c r="IO3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="P4" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="Q4" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA4" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AB4" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AC4" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL4" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN4" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AO4" s="17" t="n">
+        <v>43726</v>
+      </c>
+      <c r="IO4" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2:X4" type="list">
       <formula1>pais</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J4" type="list">
       <formula1>versao</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:U2" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:U4" type="list">
       <formula1>genero</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2409,247 +2670,247 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O1" s="20" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>48</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C3" s="21" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K3" s="22" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C5" s="21" t="n">
         <v>14</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C6" s="21" t="n">
         <v>16</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C7" s="21" t="n">
         <v>18</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="23" t="s">
         <v>51</v>
@@ -2657,336 +2918,336 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="M13" s="20" t="s">
         <v>29</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="21" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>57</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="21" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="21" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="21" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="21" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="21" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="21" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="21" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="21" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="21" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="23" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="21" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="Q25" s="23" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="21" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="Q26" s="23" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="Q27" s="23" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="21" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="21" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="Q29" s="23" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="21" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="Q30" s="23" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="21" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="21" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="21" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="Q33" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="21" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="Q34" s="23" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="21" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="Q35" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="21" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q36" s="23" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="21" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="Q37" s="23" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="21" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="Q38" s="23" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="21" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="Q39" s="23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="21" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Q40" s="23" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="21" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="Q41" s="23" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="21" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="Q42" s="23" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="21" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q43" s="23" t="s">
         <v>50</v>
@@ -2994,1085 +3255,1085 @@
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="21" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="21" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="21" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="21" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="21" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="Q48" s="23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="21" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="Q49" s="23" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="21" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="Q50" s="23" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="21" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="Q51" s="23" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="21" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="Q52" s="23" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="21" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="Q53" s="23" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="21" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="Q54" s="23" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="21" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="Q55" s="23" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="21" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="Q56" s="23" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="21" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="Q57" s="23" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="21" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="Q58" s="23" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="21" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q59" s="23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="21" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="Q60" s="23" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="21" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="Q61" s="23" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="21" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="Q62" s="23" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="21" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="Q63" s="23" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="21" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="21" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="21" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="Q66" s="23" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="21" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Q67" s="23" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="21" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="Q68" s="23" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="21" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="Q69" s="23" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="21" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="Q70" s="23" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="21" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="Q71" s="23" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="21" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="Q72" s="23" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="21" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="Q73" s="23" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="21" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q74" s="23" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="Q75" s="23" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="21" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="Q76" s="23" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="21" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="Q77" s="23" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="21" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="Q78" s="23" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="21" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="Q79" s="23" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="21" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="Q80" s="23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="21" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="Q81" s="23" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="21" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="Q82" s="23" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="21" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="Q83" s="23" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="21" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="Q84" s="23" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="21" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="Q85" s="23" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="21" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="Q86" s="23" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="21" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="Q87" s="23" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="21" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="Q88" s="23" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="21" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="Q89" s="23" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="21" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="21" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="21" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="21" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="21" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="21" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="21" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="21" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="21" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="21" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="21" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="21" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="21" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="21" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="21" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="21" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="21" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="21" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="21" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="21" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="21" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="21" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="21" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="21" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="21" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="21" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="21" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="21" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="21" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="21" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="21" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="21" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="21" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="21" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="21" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="21" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="21" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="21" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="21" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="21" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="21" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="21" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="21" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="21" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="21" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="21" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="21" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="21" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="21" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="21" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="21" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="21" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="21" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="21" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="21" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="21" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="21" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="21" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E149" s="21" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="21" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E151" s="21" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E152" s="21" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="21" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="21" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="21" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="21" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="21" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="21" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="21" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="21" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="21" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="21" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="21" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="21" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="21" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="21" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="21" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E168" s="21" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="21" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="21" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E171" s="21" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="21" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="21" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E174" s="21" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E175" s="21" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E176" s="21" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E177" s="21" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E178" s="21" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="21" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="21" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E181" s="21" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="21" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="21" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E184" s="21" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="21" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="21" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="21" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E188" s="21" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="21" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="21" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="21" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E192" s="21" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="21" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="21" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="21" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E196" s="21" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="21" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="21" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="21" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E200" s="21" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="21" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="21" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="21" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="21" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E205" s="21" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E206" s="21" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E207" s="21" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E208" s="21" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E209" s="21" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E210" s="21" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E211" s="21" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E212" s="21" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="21" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E214" s="21" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="21" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E216" s="21" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="21" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E218" s="21" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E219" s="21" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E220" s="21" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="21" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E222" s="21" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E223" s="21" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="21" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="21" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="21" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E227" s="21" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E228" s="21" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="21" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E230" s="21" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E231" s="21" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="21" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4082,72 +4343,72 @@
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E234" s="21" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E235" s="21" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E236" s="21" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E237" s="21" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="21" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E239" s="21" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E240" s="21" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="21" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E242" s="21" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E243" s="21" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="21" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E245" s="21" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E246" s="21" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="21" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -4184,80 +4445,80 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustando formato da Box - ids no arquivo categories.json
</commit_message>
<xml_diff>
--- a/xls2xml/sample/input_box_new.xlsx
+++ b/xls2xml/sample/input_box_new.xlsx
@@ -38,7 +38,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="478">
+  <si>
+    <t xml:space="preserve">uuid_box</t>
+  </si>
   <si>
     <t xml:space="preserve">Título Original</t>
   </si>
@@ -160,6 +163,9 @@
     <t xml:space="preserve">Data Início</t>
   </si>
   <si>
+    <t xml:space="preserve">b4101d20-2789-474e-9222-dc51207d45f8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 1</t>
   </si>
   <si>
@@ -229,10 +235,16 @@
     <t xml:space="preserve">E0BD54C5614CDAA111855B563DAB7A9A</t>
   </si>
   <si>
+    <t xml:space="preserve">d65ef34c-8722-4113-b039-fd147d3bbe2c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 2</t>
   </si>
   <si>
     <t xml:space="preserve">godzilla_king_otm_hd_net_evod_sub_ptbr2.ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca333c25-ed86-493f-a4b1-1defee5b8349</t>
   </si>
   <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 3</t>
@@ -1556,14 +1568,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1576,14 +1588,14 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin"/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
@@ -1671,19 +1683,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1691,11 +1707,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1846,782 +1858,795 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IP4"/>
+  <dimension ref="A1:IQ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="46.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="6.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="202.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="18.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="32" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="54.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="44.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="19.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="22.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="249" min="40" style="2" width="11.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1008" min="250" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="1009" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="24.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="43.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="202.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="18.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="54.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="44.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="22.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="250" min="41" style="2" width="11.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="251" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="1010" style="0" width="9.12"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
       <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-      <c r="BC1" s="7"/>
-      <c r="BD1" s="7"/>
-      <c r="BE1" s="7"/>
-      <c r="BF1" s="7"/>
-      <c r="BG1" s="7"/>
-      <c r="BH1" s="7"/>
-      <c r="BI1" s="7"/>
-      <c r="BJ1" s="7"/>
-      <c r="BK1" s="7"/>
-      <c r="BL1" s="7"/>
-      <c r="BM1" s="7"/>
-      <c r="BN1" s="7"/>
-      <c r="BO1" s="7"/>
-      <c r="BP1" s="7"/>
-      <c r="BQ1" s="7"/>
-      <c r="BR1" s="7"/>
-      <c r="BS1" s="7"/>
-      <c r="BT1" s="7"/>
-      <c r="BU1" s="7"/>
-      <c r="BV1" s="7"/>
-      <c r="BW1" s="7"/>
-      <c r="BX1" s="7"/>
-      <c r="BY1" s="7"/>
-      <c r="BZ1" s="7"/>
-      <c r="CA1" s="7"/>
-      <c r="CB1" s="7"/>
-      <c r="CC1" s="7"/>
-      <c r="CD1" s="7"/>
-      <c r="CE1" s="7"/>
-      <c r="CF1" s="7"/>
-      <c r="CG1" s="7"/>
-      <c r="CH1" s="7"/>
-      <c r="CI1" s="7"/>
-      <c r="CJ1" s="7"/>
-      <c r="CK1" s="7"/>
-      <c r="CL1" s="7"/>
-      <c r="CM1" s="7"/>
-      <c r="CN1" s="7"/>
-      <c r="CO1" s="7"/>
-      <c r="CP1" s="7"/>
-      <c r="CQ1" s="7"/>
-      <c r="CR1" s="7"/>
-      <c r="CS1" s="7"/>
-      <c r="CT1" s="7"/>
-      <c r="CU1" s="7"/>
-      <c r="CV1" s="7"/>
-      <c r="CW1" s="7"/>
-      <c r="CX1" s="7"/>
-      <c r="CY1" s="7"/>
-      <c r="CZ1" s="7"/>
-      <c r="DA1" s="7"/>
-      <c r="DB1" s="7"/>
-      <c r="DC1" s="7"/>
-      <c r="DD1" s="7"/>
-      <c r="DE1" s="7"/>
-      <c r="DF1" s="7"/>
-      <c r="DG1" s="7"/>
-      <c r="DH1" s="7"/>
-      <c r="DI1" s="7"/>
-      <c r="DJ1" s="7"/>
-      <c r="DK1" s="7"/>
-      <c r="DL1" s="7"/>
-      <c r="DM1" s="7"/>
-      <c r="DN1" s="7"/>
-      <c r="DO1" s="7"/>
-      <c r="DP1" s="7"/>
-      <c r="DQ1" s="7"/>
-      <c r="DR1" s="7"/>
-      <c r="DS1" s="7"/>
-      <c r="DT1" s="7"/>
-      <c r="DU1" s="7"/>
-      <c r="DV1" s="7"/>
-      <c r="DW1" s="7"/>
-      <c r="DX1" s="7"/>
-      <c r="DY1" s="7"/>
-      <c r="DZ1" s="7"/>
-      <c r="EA1" s="7"/>
-      <c r="EB1" s="7"/>
-      <c r="EC1" s="7"/>
-      <c r="ED1" s="7"/>
-      <c r="EE1" s="7"/>
-      <c r="EF1" s="7"/>
-      <c r="EG1" s="7"/>
-      <c r="EH1" s="7"/>
-      <c r="EI1" s="7"/>
-      <c r="EJ1" s="7"/>
-      <c r="EK1" s="7"/>
-      <c r="EL1" s="7"/>
-      <c r="EM1" s="7"/>
-      <c r="EN1" s="7"/>
-      <c r="EO1" s="7"/>
-      <c r="EP1" s="7"/>
-      <c r="EQ1" s="7"/>
-      <c r="ER1" s="7"/>
-      <c r="ES1" s="7"/>
-      <c r="ET1" s="7"/>
-      <c r="EU1" s="7"/>
-      <c r="EV1" s="7"/>
-      <c r="EW1" s="7"/>
-      <c r="EX1" s="7"/>
-      <c r="EY1" s="7"/>
-      <c r="EZ1" s="7"/>
-      <c r="FA1" s="7"/>
-      <c r="FB1" s="7"/>
-      <c r="FC1" s="7"/>
-      <c r="FD1" s="7"/>
-      <c r="FE1" s="7"/>
-      <c r="FF1" s="7"/>
-      <c r="FG1" s="7"/>
-      <c r="FH1" s="7"/>
-      <c r="FI1" s="7"/>
-      <c r="FJ1" s="7"/>
-      <c r="FK1" s="7"/>
-      <c r="FL1" s="7"/>
-      <c r="FM1" s="7"/>
-      <c r="FN1" s="7"/>
-      <c r="FO1" s="7"/>
-      <c r="FP1" s="7"/>
-      <c r="FQ1" s="7"/>
-      <c r="FR1" s="7"/>
-      <c r="FS1" s="7"/>
-      <c r="FT1" s="7"/>
-      <c r="FU1" s="7"/>
-      <c r="FV1" s="7"/>
-      <c r="FW1" s="7"/>
-      <c r="FX1" s="7"/>
-      <c r="FY1" s="7"/>
-      <c r="FZ1" s="7"/>
-      <c r="GA1" s="7"/>
-      <c r="GB1" s="7"/>
-      <c r="GC1" s="7"/>
-      <c r="GD1" s="7"/>
-      <c r="GE1" s="7"/>
-      <c r="GF1" s="7"/>
-      <c r="GG1" s="7"/>
-      <c r="GH1" s="7"/>
-      <c r="GI1" s="7"/>
-      <c r="GJ1" s="7"/>
-      <c r="GK1" s="7"/>
-      <c r="GL1" s="7"/>
-      <c r="GM1" s="7"/>
-      <c r="GN1" s="7"/>
-      <c r="GO1" s="7"/>
-      <c r="GP1" s="7"/>
-      <c r="GQ1" s="7"/>
-      <c r="GR1" s="7"/>
-      <c r="GS1" s="7"/>
-      <c r="GT1" s="7"/>
-      <c r="GU1" s="7"/>
-      <c r="GV1" s="7"/>
-      <c r="GW1" s="7"/>
-      <c r="GX1" s="7"/>
-      <c r="GY1" s="7"/>
-      <c r="GZ1" s="7"/>
-      <c r="HA1" s="7"/>
-      <c r="HB1" s="7"/>
-      <c r="HC1" s="7"/>
-      <c r="HD1" s="7"/>
-      <c r="HE1" s="7"/>
-      <c r="HF1" s="7"/>
-      <c r="HG1" s="7"/>
-      <c r="HH1" s="7"/>
-      <c r="HI1" s="7"/>
-      <c r="HJ1" s="7"/>
-      <c r="HK1" s="7"/>
-      <c r="HL1" s="7"/>
-      <c r="HM1" s="7"/>
-      <c r="HN1" s="7"/>
-      <c r="HO1" s="7"/>
-      <c r="HP1" s="7"/>
-      <c r="HQ1" s="7"/>
-      <c r="HR1" s="7"/>
-      <c r="HS1" s="7"/>
-      <c r="HT1" s="7"/>
-      <c r="HU1" s="7"/>
-      <c r="HV1" s="7"/>
-      <c r="HW1" s="7"/>
-      <c r="HX1" s="7"/>
-      <c r="HY1" s="7"/>
-      <c r="HZ1" s="7"/>
-      <c r="IA1" s="7"/>
-      <c r="IB1" s="7"/>
-      <c r="IC1" s="7"/>
-      <c r="ID1" s="7"/>
-      <c r="IE1" s="7"/>
-      <c r="IF1" s="7"/>
-      <c r="IG1" s="7"/>
-      <c r="IH1" s="7"/>
-      <c r="II1" s="7"/>
-      <c r="IJ1" s="7"/>
-      <c r="IK1" s="7"/>
-      <c r="IL1" s="7"/>
-      <c r="IM1" s="7"/>
-      <c r="IN1" s="7"/>
-      <c r="IO1" s="7"/>
+      <c r="AO1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
+      <c r="DE1" s="8"/>
+      <c r="DF1" s="8"/>
+      <c r="DG1" s="8"/>
+      <c r="DH1" s="8"/>
+      <c r="DI1" s="8"/>
+      <c r="DJ1" s="8"/>
+      <c r="DK1" s="8"/>
+      <c r="DL1" s="8"/>
+      <c r="DM1" s="8"/>
+      <c r="DN1" s="8"/>
+      <c r="DO1" s="8"/>
+      <c r="DP1" s="8"/>
+      <c r="DQ1" s="8"/>
+      <c r="DR1" s="8"/>
+      <c r="DS1" s="8"/>
+      <c r="DT1" s="8"/>
+      <c r="DU1" s="8"/>
+      <c r="DV1" s="8"/>
+      <c r="DW1" s="8"/>
+      <c r="DX1" s="8"/>
+      <c r="DY1" s="8"/>
+      <c r="DZ1" s="8"/>
+      <c r="EA1" s="8"/>
+      <c r="EB1" s="8"/>
+      <c r="EC1" s="8"/>
+      <c r="ED1" s="8"/>
+      <c r="EE1" s="8"/>
+      <c r="EF1" s="8"/>
+      <c r="EG1" s="8"/>
+      <c r="EH1" s="8"/>
+      <c r="EI1" s="8"/>
+      <c r="EJ1" s="8"/>
+      <c r="EK1" s="8"/>
+      <c r="EL1" s="8"/>
+      <c r="EM1" s="8"/>
+      <c r="EN1" s="8"/>
+      <c r="EO1" s="8"/>
+      <c r="EP1" s="8"/>
+      <c r="EQ1" s="8"/>
+      <c r="ER1" s="8"/>
+      <c r="ES1" s="8"/>
+      <c r="ET1" s="8"/>
+      <c r="EU1" s="8"/>
+      <c r="EV1" s="8"/>
+      <c r="EW1" s="8"/>
+      <c r="EX1" s="8"/>
+      <c r="EY1" s="8"/>
+      <c r="EZ1" s="8"/>
+      <c r="FA1" s="8"/>
+      <c r="FB1" s="8"/>
+      <c r="FC1" s="8"/>
+      <c r="FD1" s="8"/>
+      <c r="FE1" s="8"/>
+      <c r="FF1" s="8"/>
+      <c r="FG1" s="8"/>
+      <c r="FH1" s="8"/>
+      <c r="FI1" s="8"/>
+      <c r="FJ1" s="8"/>
+      <c r="FK1" s="8"/>
+      <c r="FL1" s="8"/>
+      <c r="FM1" s="8"/>
+      <c r="FN1" s="8"/>
+      <c r="FO1" s="8"/>
+      <c r="FP1" s="8"/>
+      <c r="FQ1" s="8"/>
+      <c r="FR1" s="8"/>
+      <c r="FS1" s="8"/>
+      <c r="FT1" s="8"/>
+      <c r="FU1" s="8"/>
+      <c r="FV1" s="8"/>
+      <c r="FW1" s="8"/>
+      <c r="FX1" s="8"/>
+      <c r="FY1" s="8"/>
+      <c r="FZ1" s="8"/>
+      <c r="GA1" s="8"/>
+      <c r="GB1" s="8"/>
+      <c r="GC1" s="8"/>
+      <c r="GD1" s="8"/>
+      <c r="GE1" s="8"/>
+      <c r="GF1" s="8"/>
+      <c r="GG1" s="8"/>
+      <c r="GH1" s="8"/>
+      <c r="GI1" s="8"/>
+      <c r="GJ1" s="8"/>
+      <c r="GK1" s="8"/>
+      <c r="GL1" s="8"/>
+      <c r="GM1" s="8"/>
+      <c r="GN1" s="8"/>
+      <c r="GO1" s="8"/>
+      <c r="GP1" s="8"/>
+      <c r="GQ1" s="8"/>
+      <c r="GR1" s="8"/>
+      <c r="GS1" s="8"/>
+      <c r="GT1" s="8"/>
+      <c r="GU1" s="8"/>
+      <c r="GV1" s="8"/>
+      <c r="GW1" s="8"/>
+      <c r="GX1" s="8"/>
+      <c r="GY1" s="8"/>
+      <c r="GZ1" s="8"/>
+      <c r="HA1" s="8"/>
+      <c r="HB1" s="8"/>
+      <c r="HC1" s="8"/>
+      <c r="HD1" s="8"/>
+      <c r="HE1" s="8"/>
+      <c r="HF1" s="8"/>
+      <c r="HG1" s="8"/>
+      <c r="HH1" s="8"/>
+      <c r="HI1" s="8"/>
+      <c r="HJ1" s="8"/>
+      <c r="HK1" s="8"/>
+      <c r="HL1" s="8"/>
+      <c r="HM1" s="8"/>
+      <c r="HN1" s="8"/>
+      <c r="HO1" s="8"/>
+      <c r="HP1" s="8"/>
+      <c r="HQ1" s="8"/>
+      <c r="HR1" s="8"/>
+      <c r="HS1" s="8"/>
+      <c r="HT1" s="8"/>
+      <c r="HU1" s="8"/>
+      <c r="HV1" s="8"/>
+      <c r="HW1" s="8"/>
+      <c r="HX1" s="8"/>
+      <c r="HY1" s="8"/>
+      <c r="HZ1" s="8"/>
+      <c r="IA1" s="8"/>
+      <c r="IB1" s="8"/>
+      <c r="IC1" s="8"/>
+      <c r="ID1" s="8"/>
+      <c r="IE1" s="8"/>
+      <c r="IF1" s="8"/>
+      <c r="IG1" s="8"/>
+      <c r="IH1" s="8"/>
+      <c r="II1" s="8"/>
+      <c r="IJ1" s="8"/>
+      <c r="IK1" s="8"/>
+      <c r="IL1" s="8"/>
+      <c r="IM1" s="8"/>
+      <c r="IN1" s="8"/>
+      <c r="IO1" s="8"/>
       <c r="IP1" s="8"/>
+      <c r="IQ1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
+      <c r="A2" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="E2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>7899119860</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>57639</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="Q2" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="R2" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AC2" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AD2" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO2" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AP2" s="17" t="n">
+        <v>43726</v>
+      </c>
+      <c r="IP2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="I3" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="K3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="Q3" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="R3" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB3" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AC3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AD3" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK3" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM3" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AP3" s="17" t="n">
+        <v>43726</v>
+      </c>
+      <c r="IP3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="K4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="L4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="M4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="P2" s="13" t="n">
+      <c r="Q4" s="13" t="n">
         <v>1000000</v>
       </c>
-      <c r="Q2" s="14" t="n">
+      <c r="R4" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="1" t="n">
+      <c r="S4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="X4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AA2" s="16" t="n">
+      <c r="Z4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" s="16" t="n">
         <v>0.0914467592592593</v>
       </c>
-      <c r="AB2" s="17" t="n">
+      <c r="AC4" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AC2" s="17" t="n">
+      <c r="AD4" s="17" t="n">
         <v>44092</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="1" t="n">
+      <c r="AF4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="AH2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ2" s="2" t="n">
+      <c r="AI4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK4" s="2" t="n">
         <v>144591928</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM4" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AN4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AL2" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN2" s="17" t="n">
+      <c r="AO4" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AO2" s="17" t="n">
+      <c r="AP4" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IO2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>7899119860</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>57639</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="P3" s="13" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="Q3" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA3" s="16" t="n">
-        <v>0.0914467592592593</v>
-      </c>
-      <c r="AB3" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AC3" s="17" t="n">
-        <v>44092</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG3" s="1" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ3" s="2" t="n">
-        <v>144591928</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL3" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN3" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AO3" s="17" t="n">
-        <v>43726</v>
-      </c>
-      <c r="IO3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>7899119860</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>57639</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="P4" s="13" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="Q4" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA4" s="16" t="n">
-        <v>0.0914467592592593</v>
-      </c>
-      <c r="AB4" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AC4" s="17" t="n">
-        <v>44092</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG4" s="1" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ4" s="2" t="n">
-        <v>144591928</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL4" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN4" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AO4" s="17" t="n">
-        <v>43726</v>
-      </c>
-      <c r="IO4" s="1"/>
+      <c r="IP4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2:X4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y2:Y4" type="list">
       <formula1>pais</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K4" type="list">
       <formula1>versao</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:U4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U2:V4" type="list">
       <formula1>genero</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N15" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O15" type="list">
       <formula1>Categoria</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2670,1745 +2695,1745 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C2" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C3" s="21" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K3" s="22" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C5" s="21" t="n">
         <v>14</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C6" s="21" t="n">
         <v>16</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C7" s="21" t="n">
         <v>18</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="21" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="21" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="21" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="21" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="21" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="21" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="21" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="21" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="21" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="21" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="21" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="Q24" s="23" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="21" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="Q25" s="23" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="21" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="Q26" s="23" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="Q27" s="23" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="21" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="Q29" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="Q30" s="23" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="21" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="21" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="21" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="Q33" s="23" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="21" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="Q34" s="23" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="21" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="Q35" s="23" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="21" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="Q36" s="23" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="21" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q37" s="23" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="21" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="Q38" s="23" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="21" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="Q39" s="23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="21" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="Q40" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="21" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="Q41" s="23" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="21" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="Q42" s="23" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="21" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="Q43" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="21" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="21" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="21" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="21" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="Q48" s="23" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="21" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="Q49" s="23" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="21" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="Q50" s="23" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="21" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="Q51" s="23" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="21" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q52" s="23" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="21" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="Q53" s="23" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="21" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="Q54" s="23" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="21" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Q55" s="23" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="21" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="Q56" s="23" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="21" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="Q57" s="23" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="21" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="Q58" s="23" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="21" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="Q59" s="23" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="21" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="Q60" s="23" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="21" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="Q61" s="23" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="21" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="Q62" s="23" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="21" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="Q63" s="23" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="21" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="21" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="21" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="Q66" s="23" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="21" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="Q67" s="23" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="21" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="Q68" s="23" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="21" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="Q69" s="23" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="21" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="Q70" s="23" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="21" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="Q71" s="23" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="21" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="Q72" s="23" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="21" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="Q73" s="23" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="21" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="Q74" s="23" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="21" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="Q75" s="23" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="21" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q76" s="23" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="21" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="Q77" s="23" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="21" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="Q78" s="23" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="21" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="Q79" s="23" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="Q80" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="21" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="Q81" s="23" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="21" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="Q82" s="23" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="21" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="Q83" s="23" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="21" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="Q84" s="23" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="21" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="Q85" s="23" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="21" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="Q86" s="23" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="21" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="Q87" s="23" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="21" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="Q88" s="23" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="21" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="Q89" s="23" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="21" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="21" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="21" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="21" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="21" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="21" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="21" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="21" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="21" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="21" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="21" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="21" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="21" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="21" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="21" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="21" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="21" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="21" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="21" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="21" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="21" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="21" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="21" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="21" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="21" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="21" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="21" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="21" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="21" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="21" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="21" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="21" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="21" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="21" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="21" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="21" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="21" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="21" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="21" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="21" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="21" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="21" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="21" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="21" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="21" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="21" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="21" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="21" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="21" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="21" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="21" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="21" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="21" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="21" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="21" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="21" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="21" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="21" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="21" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E149" s="21" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="21" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E151" s="21" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E152" s="21" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="21" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="21" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="21" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="21" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="21" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="21" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="21" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="21" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="21" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="21" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="21" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="21" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="21" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="21" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="21" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E168" s="21" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="21" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="21" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E171" s="21" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="21" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="21" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E174" s="21" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E175" s="21" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E176" s="21" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E177" s="21" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E178" s="21" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="21" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="21" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E181" s="21" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="21" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="21" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E184" s="21" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="21" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="21" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="21" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E188" s="21" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="21" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="21" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="21" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E192" s="21" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="21" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="21" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="21" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E196" s="21" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="21" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="21" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="21" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E200" s="21" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="21" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="21" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="21" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="21" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E205" s="21" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E206" s="21" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E207" s="21" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E208" s="21" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E209" s="21" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E210" s="21" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E211" s="21" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E212" s="21" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="21" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E214" s="21" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="21" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E216" s="21" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="21" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E218" s="21" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E219" s="21" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E220" s="21" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="21" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E222" s="21" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E223" s="21" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="21" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="21" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="21" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E227" s="21" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E228" s="21" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="21" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E230" s="21" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E231" s="21" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="21" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E233" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E234" s="21" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E235" s="21" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E236" s="21" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E237" s="21" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="21" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E239" s="21" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E240" s="21" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="21" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E242" s="21" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E243" s="21" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="21" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E245" s="21" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E246" s="21" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="21" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -4445,80 +4470,80 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Box - acertando prefixos de diretorios e ids de imagens
</commit_message>
<xml_diff>
--- a/xls2xml/sample/input_box_new.xlsx
+++ b/xls2xml/sample/input_box_new.xlsx
@@ -38,11 +38,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="489">
   <si>
     <t xml:space="preserve">uuid_box</t>
   </si>
   <si>
+    <t xml:space="preserve">uuid_poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid_landscape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid_thumb</t>
+  </si>
+  <si>
     <t xml:space="preserve">Título Original</t>
   </si>
   <si>
@@ -166,6 +175,15 @@
     <t xml:space="preserve">b4101d20-2789-474e-9222-dc51207d45f8</t>
   </si>
   <si>
+    <t xml:space="preserve">c0c55502-eb14-4997-8ee9-aa4b09c2d4a6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70156e26-6f1c-4bbc-9f27-e144916e7f0c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23051aa2-9857-44f1-8b5e-82df6b683a88</t>
+  </si>
+  <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 1</t>
   </si>
   <si>
@@ -238,6 +256,15 @@
     <t xml:space="preserve">d65ef34c-8722-4113-b039-fd147d3bbe2c</t>
   </si>
   <si>
+    <t xml:space="preserve">18ef3b37-da6c-4b81-b7be-0ee352b7748d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8b4736ae-a375-4d35-937e-0facd33c65d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fb4516ac-6f1e-4851-853d-dd575a7e4de0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 2</t>
   </si>
   <si>
@@ -245,6 +272,12 @@
   </si>
   <si>
     <t xml:space="preserve">ca333c25-ed86-493f-a4b1-1defee5b8349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fc5ae815-f7ba-4119-aa04-56de8b934996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7d3be747-0bd9-4046-8296-10cb74883c75</t>
   </si>
   <si>
     <t xml:space="preserve">Godzilla: King Of The Monsters 3</t>
@@ -1858,79 +1891,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IQ4"/>
+  <dimension ref="A1:IT4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="202.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="18.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="54.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="44.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="19.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="22.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="250" min="41" style="2" width="11.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="251" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="1010" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="24.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="46.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="43.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="21.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="6.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="202.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="21.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="54.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="2" width="44.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="2" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="2" width="22.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="253" min="44" style="2" width="11.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="254" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1013" style="0" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -1939,19 +1972,19 @@
       <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="5" t="s">
@@ -2011,13 +2044,13 @@
       <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AL1" s="6" t="s">
@@ -2026,18 +2059,24 @@
       <c r="AM1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
+      <c r="AP1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="AT1" s="8"/>
       <c r="AU1" s="8"/>
       <c r="AV1" s="8"/>
@@ -2243,410 +2282,440 @@
       <c r="IN1" s="8"/>
       <c r="IO1" s="8"/>
       <c r="IP1" s="8"/>
-      <c r="IQ1" s="9"/>
+      <c r="IQ1" s="8"/>
+      <c r="IR1" s="8"/>
+      <c r="IS1" s="8"/>
+      <c r="IT1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="H2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="1" t="n">
+      <c r="I2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>7899119860</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="1" t="n">
+      <c r="K2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>57639</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="1" t="n">
+      <c r="M2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="Q2" s="13" t="n">
+      <c r="T2" s="13" t="n">
         <v>1000000</v>
       </c>
-      <c r="R2" s="14" t="n">
+      <c r="U2" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="1" t="n">
+      <c r="V2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="X2" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" s="16" t="n">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="16" t="n">
         <v>0.0914467592592593</v>
       </c>
-      <c r="AC2" s="17" t="n">
+      <c r="AF2" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AD2" s="17" t="n">
+      <c r="AG2" s="17" t="n">
         <v>44092</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH2" s="1" t="n">
+      <c r="AH2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK2" s="2" t="n">
+      <c r="AL2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN2" s="2" t="n">
         <v>144591928</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM2" s="18" t="n">
+      <c r="AO2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP2" s="18" t="n">
         <v>0.00166666666666667</v>
       </c>
-      <c r="AN2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO2" s="17" t="n">
+      <c r="AQ2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AP2" s="17" t="n">
+      <c r="AS2" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IP2" s="1"/>
+      <c r="IS2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="T3" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="U3" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AF3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AG3" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>7899119860</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>57639</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="Q3" s="13" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="R3" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB3" s="16" t="n">
-        <v>0.0914467592592593</v>
-      </c>
-      <c r="AC3" s="17" t="n">
+      <c r="AK3" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN3" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP3" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR3" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AD3" s="17" t="n">
-        <v>44092</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH3" s="1" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK3" s="2" t="n">
-        <v>144591928</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM3" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO3" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AP3" s="17" t="n">
+      <c r="AS3" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IP3" s="1"/>
+      <c r="IS3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="T4" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="U4" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE4" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AF4" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AG4" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="AM4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>7899119860</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>57639</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="Q4" s="13" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="R4" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T4" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="16" t="n">
-        <v>0.0914467592592593</v>
-      </c>
-      <c r="AC4" s="17" t="n">
+      <c r="AN4" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP4" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR4" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AD4" s="17" t="n">
-        <v>44092</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH4" s="1" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK4" s="2" t="n">
-        <v>144591928</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM4" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO4" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AP4" s="17" t="n">
+      <c r="AS4" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IP4" s="1"/>
+      <c r="IS4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y2:Y4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB2:AB4" type="list">
       <formula1>pais</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N4" type="list">
       <formula1>versao</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U2:V4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2:Y4" type="list">
       <formula1>genero</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O15" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2:R15" type="list">
       <formula1>Categoria</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2695,1745 +2764,1745 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C2" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C3" s="21" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="K3" s="22" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C5" s="21" t="n">
         <v>14</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C6" s="21" t="n">
         <v>16</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C7" s="21" t="n">
         <v>18</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="21" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="21" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="21" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="21" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="21" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="21" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="21" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="21" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="21" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="21" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="21" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="21" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="Q24" s="23" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="21" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="Q25" s="23" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="21" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="Q26" s="23" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="21" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="Q27" s="23" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="21" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="21" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="Q29" s="23" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="21" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="Q30" s="23" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="21" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="21" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="21" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="Q33" s="23" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="21" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="Q34" s="23" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="21" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="Q35" s="23" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="21" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="Q36" s="23" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="21" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="Q37" s="23" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="21" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="Q38" s="23" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="21" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="Q39" s="23" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="21" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="Q40" s="23" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="21" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="Q41" s="23" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="21" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="Q42" s="23" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="21" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="Q43" s="23" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="21" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="21" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="21" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="21" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="21" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="Q48" s="23" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="21" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="Q49" s="23" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="21" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="Q50" s="23" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="21" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="Q51" s="23" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="21" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="Q52" s="23" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="21" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="Q53" s="23" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="21" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="Q54" s="23" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="21" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="Q55" s="23" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="21" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="Q56" s="23" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="21" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="Q57" s="23" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="21" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="Q58" s="23" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="21" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="Q59" s="23" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="21" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="Q60" s="23" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="21" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="Q61" s="23" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="21" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="Q62" s="23" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="21" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="Q63" s="23" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="21" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="21" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="21" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="Q66" s="23" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="21" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="Q67" s="23" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="21" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="Q68" s="23" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="21" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="Q69" s="23" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="21" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="Q70" s="23" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="21" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="Q71" s="23" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="21" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="Q72" s="23" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="21" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="Q73" s="23" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="21" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="Q74" s="23" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="21" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="Q75" s="23" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="21" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="Q76" s="23" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="21" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="Q77" s="23" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="21" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="Q78" s="23" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="21" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="Q79" s="23" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="21" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="Q80" s="23" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="21" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="Q81" s="23" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="21" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="Q82" s="23" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="21" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="Q83" s="23" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="21" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="Q84" s="23" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="21" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="Q85" s="23" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="21" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="Q86" s="23" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="21" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="Q87" s="23" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="21" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="Q88" s="23" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="21" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="Q89" s="23" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="21" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="21" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="21" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="21" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="21" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="21" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="21" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="21" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="21" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="21" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="21" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="21" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="21" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="21" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="21" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="21" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="21" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="21" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="21" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="21" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="21" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="21" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="21" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="21" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="21" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="21" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="21" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="21" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="21" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="21" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="21" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="21" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="21" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="21" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="21" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="21" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="21" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="21" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="21" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="21" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="21" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="21" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="21" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="21" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="21" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="21" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="21" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="21" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="21" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="21" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="21" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="21" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="21" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="21" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="21" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="21" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="21" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="21" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="21" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E149" s="21" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="21" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E151" s="21" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E152" s="21" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="21" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="21" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="21" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="21" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="21" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="21" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="21" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="21" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="21" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="21" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="21" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="21" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="21" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="21" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="21" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E168" s="21" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="21" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="21" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E171" s="21" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="21" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="21" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E174" s="21" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E175" s="21" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E176" s="21" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E177" s="21" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E178" s="21" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="21" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="21" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E181" s="21" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="21" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="21" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E184" s="21" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="21" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="21" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="21" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E188" s="21" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="21" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="21" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="21" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E192" s="21" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="21" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="21" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="21" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E196" s="21" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="21" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="21" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="21" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E200" s="21" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="21" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="21" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="21" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="21" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E205" s="21" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E206" s="21" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E207" s="21" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E208" s="21" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E209" s="21" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E210" s="21" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E211" s="21" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E212" s="21" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="21" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E214" s="21" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="21" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E216" s="21" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="21" t="s">
-        <v>435</v>
+        <v>446</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E218" s="21" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E219" s="21" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E220" s="21" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="21" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E222" s="21" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E223" s="21" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="21" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="21" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="21" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E227" s="21" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E228" s="21" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="21" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E230" s="21" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E231" s="21" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="21" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E233" s="21" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E234" s="21" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E235" s="21" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E236" s="21" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E237" s="21" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="21" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E239" s="21" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E240" s="21" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="21" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E242" s="21" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E243" s="21" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="21" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E245" s="21" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E246" s="21" t="s">
-        <v>463</v>
+        <v>474</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="21" t="s">
-        <v>464</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -4470,80 +4539,80 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>465</v>
+        <v>476</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>466</v>
+        <v>477</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>467</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>468</v>
+        <v>479</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Box - corrigindo bug de arrays de elementos (aparecia so o primeiro)
</commit_message>
<xml_diff>
--- a/xls2xml/sample/input_box_new.xlsx
+++ b/xls2xml/sample/input_box_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,11 +38,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="497">
   <si>
     <t xml:space="preserve">uuid_box</t>
   </si>
   <si>
+    <t xml:space="preserve">uuid_trailer</t>
+  </si>
+  <si>
     <t xml:space="preserve">uuid_poster</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
     <t xml:space="preserve">b4101d20-2789-474e-9222-dc51207d45f8</t>
   </si>
   <si>
+    <t xml:space="preserve">237e4936-6a73-42ef-880f-336e6ade2bb8</t>
+  </si>
+  <si>
     <t xml:space="preserve">c0c55502-eb14-4997-8ee9-aa4b09c2d4a6</t>
   </si>
   <si>
@@ -256,6 +262,9 @@
     <t xml:space="preserve">d65ef34c-8722-4113-b039-fd147d3bbe2c</t>
   </si>
   <si>
+    <t xml:space="preserve">f68933b1-3745-4ef4-9617-fabb34fa9f01</t>
+  </si>
+  <si>
     <t xml:space="preserve">18ef3b37-da6c-4b81-b7be-0ee352b7748d</t>
   </si>
   <si>
@@ -274,6 +283,9 @@
     <t xml:space="preserve">ca333c25-ed86-493f-a4b1-1defee5b8349</t>
   </si>
   <si>
+    <t xml:space="preserve">b61c9269-f918-4f90-9550-d795b58e7281</t>
+  </si>
+  <si>
     <t xml:space="preserve">fc5ae815-f7ba-4119-aa04-56de8b934996</t>
   </si>
   <si>
@@ -1505,6 +1517,18 @@
   </si>
   <si>
     <t xml:space="preserve">por:Aventura|eng:Adventure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d7d4b94e-6055-4400-8325-c7f754830573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">por:Show|eng:Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2f7c576a-7212-4af7-ac90-cbd6df1e5f94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">por:Música|eng:Music</t>
   </si>
 </sst>
 </file>
@@ -1891,54 +1915,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IT4"/>
+  <dimension ref="A1:IU4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="34.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="46.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="21.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="6.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="202.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="54.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="2" width="44.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="2" width="19.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="2" width="22.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="253" min="44" style="2" width="11.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="254" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1013" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="24.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="46.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="43.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="202.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="18.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="37" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="21.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="54.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="2" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="2" width="44.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="2" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="2" width="22.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="254" min="45" style="2" width="11.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="255" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1014" style="0" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,10 +1978,10 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -1966,7 +1990,7 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -1981,13 +2005,13 @@
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="5" t="s">
@@ -2053,7 +2077,7 @@
       <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="6" t="s">
@@ -2068,16 +2092,18 @@
       <c r="AP1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="7" t="s">
         <v>43</v>
       </c>
       <c r="AS1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AT1" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="AU1" s="8"/>
       <c r="AV1" s="8"/>
       <c r="AW1" s="8"/>
@@ -2285,437 +2311,447 @@
       <c r="IQ1" s="8"/>
       <c r="IR1" s="8"/>
       <c r="IS1" s="8"/>
-      <c r="IT1" s="9"/>
+      <c r="IT1" s="8"/>
+      <c r="IU1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>49</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="I2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>7899119860</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>57639</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P2" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="R2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="T2" s="13" t="n">
+      <c r="U2" s="13" t="n">
         <v>1000000</v>
       </c>
-      <c r="U2" s="14" t="n">
+      <c r="V2" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W2" s="1" t="n">
+      <c r="W2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="16" t="n">
+      <c r="AD2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF2" s="16" t="n">
         <v>0.0914467592592593</v>
       </c>
-      <c r="AF2" s="17" t="n">
+      <c r="AG2" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AG2" s="17" t="n">
+      <c r="AH2" s="17" t="n">
         <v>44092</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="AI2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK2" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL2" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AM2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN2" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" s="2" t="n">
         <v>144591928</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ2" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AP2" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR2" s="17" t="n">
+      <c r="AS2" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AS2" s="17" t="n">
+      <c r="AT2" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IS2" s="1"/>
+      <c r="IT2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>7899119860</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>57639</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="U3" s="13" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="V3" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="16" t="n">
+        <v>0.0914467592592593</v>
+      </c>
+      <c r="AG3" s="17" t="n">
+        <v>43713</v>
+      </c>
+      <c r="AH3" s="17" t="n">
+        <v>44092</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="AO3" s="2" t="n">
+        <v>144591928</v>
+      </c>
+      <c r="AP3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>7899119860</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>57639</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="T3" s="13" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="U3" s="14" t="n">
-        <v>9</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W3" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC3" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE3" s="16" t="n">
-        <v>0.0914467592592593</v>
-      </c>
-      <c r="AF3" s="17" t="n">
+      <c r="AQ3" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS3" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AG3" s="17" t="n">
-        <v>44092</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK3" s="1" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN3" s="2" t="n">
-        <v>144591928</v>
-      </c>
-      <c r="AO3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP3" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR3" s="17" t="n">
-        <v>43713</v>
-      </c>
-      <c r="AS3" s="17" t="n">
+      <c r="AT3" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IS3" s="1"/>
+      <c r="IT3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" s="1" t="n">
+      <c r="K4" s="1" t="n">
         <v>7899119860</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>57639</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="O4" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P4" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="1" t="n">
+      <c r="R4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="T4" s="13" t="n">
+      <c r="U4" s="13" t="n">
         <v>1000000</v>
       </c>
-      <c r="U4" s="14" t="n">
+      <c r="V4" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" s="1" t="n">
+      <c r="W4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="Y4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AE4" s="16" t="n">
+      <c r="AD4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF4" s="16" t="n">
         <v>0.0914467592592593</v>
       </c>
-      <c r="AF4" s="17" t="n">
+      <c r="AG4" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AG4" s="17" t="n">
+      <c r="AH4" s="17" t="n">
         <v>44092</v>
       </c>
-      <c r="AH4" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="AI4" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK4" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL4" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="AL4" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AM4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN4" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" s="2" t="n">
         <v>144591928</v>
       </c>
-      <c r="AO4" s="2" t="s">
+      <c r="AP4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ4" s="18" t="n">
+        <v>0.00166666666666667</v>
+      </c>
+      <c r="AR4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AP4" s="18" t="n">
-        <v>0.00166666666666667</v>
-      </c>
-      <c r="AQ4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR4" s="17" t="n">
+      <c r="AS4" s="17" t="n">
         <v>43713</v>
       </c>
-      <c r="AS4" s="17" t="n">
+      <c r="AT4" s="17" t="n">
         <v>43726</v>
       </c>
-      <c r="IS4" s="1"/>
+      <c r="IT4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB2:AB4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC2:AC4" type="list">
       <formula1>pais</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O4" type="list">
       <formula1>versao</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2:Y4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y2:Z4" type="list">
       <formula1>genero</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2:R15" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:S15" type="list">
       <formula1>Categoria</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2764,1745 +2800,1745 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C2" s="21" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C3" s="21" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K3" s="22" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C5" s="21" t="n">
         <v>14</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C6" s="21" t="n">
         <v>16</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C7" s="21" t="n">
         <v>18</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="21" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="21" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="21" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="21" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="21" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="21" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="21" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="21" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="21" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="Q24" s="23" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="Q25" s="23" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="21" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="Q26" s="23" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="21" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="Q27" s="23" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="21" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="21" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="Q29" s="23" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="21" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q30" s="23" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="21" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="21" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="21" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="Q33" s="23" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="21" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="Q34" s="23" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="21" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="Q35" s="23" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="21" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="Q36" s="23" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="21" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="Q37" s="23" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="Q38" s="23" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="21" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="Q39" s="23" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="21" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="Q40" s="23" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="21" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="Q41" s="23" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="21" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="Q42" s="23" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="21" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="Q43" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="21" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q44" s="23" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="21" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="Q45" s="23" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="21" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="Q46" s="23" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="21" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Q47" s="23" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="21" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="Q48" s="23" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="21" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="Q49" s="23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="21" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="Q50" s="23" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="21" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="Q51" s="23" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="21" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="Q52" s="23" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="21" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="Q53" s="23" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="21" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="Q54" s="23" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="21" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="Q55" s="23" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="21" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="Q56" s="23" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="21" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="Q57" s="23" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="21" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="Q58" s="23" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="21" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="Q59" s="23" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="21" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="Q60" s="23" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="21" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="Q61" s="23" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="21" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="Q62" s="23" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="21" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="Q63" s="23" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="21" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="Q64" s="23" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="21" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="Q65" s="23" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="21" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="Q66" s="23" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="21" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q67" s="23" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="21" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="Q68" s="23" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="21" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="Q69" s="23" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="21" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Q70" s="23" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="21" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="Q71" s="23" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="21" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="Q72" s="23" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="21" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="Q73" s="23" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="21" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="Q74" s="23" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="21" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="Q75" s="23" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="21" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="Q76" s="23" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="21" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="Q77" s="23" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="21" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="Q78" s="23" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="21" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="Q79" s="23" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="21" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="Q80" s="23" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="21" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="Q81" s="23" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="21" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="Q82" s="23" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="21" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="Q83" s="23" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="21" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="Q84" s="23" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="21" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="Q85" s="23" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="21" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="Q86" s="23" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="21" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="Q87" s="23" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="21" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="Q88" s="23" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="21" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="Q89" s="23" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="21" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="21" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="21" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="21" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="21" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="21" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="21" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="21" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="21" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="21" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="21" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="21" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="21" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="21" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="21" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="21" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="21" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="21" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="21" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="21" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="21" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="21" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="21" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="21" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="21" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="21" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="21" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="21" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="21" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="21" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="21" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="21" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="21" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="21" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="21" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="21" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="21" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="21" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="21" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="21" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="21" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="21" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="21" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="21" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="21" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="21" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="21" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="21" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="21" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="21" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="21" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="21" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="21" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="21" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="21" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="21" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="21" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="21" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="21" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E149" s="21" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="21" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E151" s="21" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E152" s="21" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="21" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="21" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="21" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="21" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="21" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="21" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="21" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="21" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="21" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="21" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="21" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="21" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="21" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="21" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="21" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E168" s="21" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="21" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="21" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E171" s="21" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="21" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="21" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E174" s="21" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E175" s="21" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E176" s="21" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E177" s="21" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E178" s="21" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="21" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="21" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E181" s="21" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="21" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="21" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E184" s="21" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="21" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="21" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="21" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E188" s="21" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="21" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="21" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="21" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E192" s="21" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="21" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="21" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="21" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E196" s="21" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="21" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="21" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="21" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E200" s="21" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="21" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="21" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="21" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="21" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E205" s="21" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E206" s="21" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E207" s="21" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E208" s="21" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E209" s="21" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E210" s="21" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E211" s="21" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E212" s="21" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="21" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E214" s="21" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="21" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E216" s="21" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="21" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E218" s="21" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E219" s="21" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E220" s="21" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="21" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E222" s="21" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E223" s="21" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="21" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="21" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="21" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E227" s="21" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E228" s="21" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="21" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E230" s="21" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E231" s="21" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="21" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E233" s="21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E234" s="21" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E235" s="21" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E236" s="21" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E237" s="21" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="21" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E239" s="21" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E240" s="21" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="21" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E242" s="21" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E243" s="21" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="21" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E245" s="21" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E246" s="21" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="21" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -4521,9 +4557,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4539,80 +4575,132 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>486</v>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>